<commit_message>
updated with 8/2 data
</commit_message>
<xml_diff>
--- a/data/2017-07-30-pacific-oyster-larvae/2017-07-29-Spawning-Calculations.xlsx
+++ b/data/2017-07-30-pacific-oyster-larvae/2017-07-29-Spawning-Calculations.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yaaminivenkataraman/Desktop/spawning/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yaaminivenkataraman/Documents/project-oyster-oa/data/2017-07-30-pacific-oyster-larvae/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14540" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14540" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="sex" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="192">
   <si>
     <t>Sex</t>
   </si>
@@ -627,11 +627,17 @@
   <si>
     <t>Volume Added</t>
   </si>
+  <si>
+    <t>Average hatch rate, excluding high outliers</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -747,7 +753,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -778,6 +784,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="25" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="34">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -20876,8 +20883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22154,6 +22161,9 @@
         <f>AVERAGE(M26,M24,M23,M22,M21,M20,M18,M17,M15,M14,M13,M12,M11,M10,M9,M8,M7,M6,M5,M4,M3,M2)</f>
         <v>0.47991437564519612</v>
       </c>
+      <c r="N28" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
@@ -22169,9 +22179,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScale="102" workbookViewId="0"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="102" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -22229,7 +22241,7 @@
       <c r="C2" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="18">
         <f>SUM(hatching!L2:L7)</f>
         <v>516326.03174603183</v>
       </c>
@@ -22250,7 +22262,7 @@
       <c r="J2" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="18">
         <f>D2/5</f>
         <v>103265.20634920636</v>
       </c>
@@ -22265,7 +22277,7 @@
       <c r="C3" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="18">
         <f>SUM(hatching!L8:L13)</f>
         <v>515897.77777777775</v>
       </c>
@@ -22286,7 +22298,7 @@
       <c r="J3" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="18">
         <f>D3/5</f>
         <v>103179.55555555555</v>
       </c>
@@ -22301,7 +22313,7 @@
       <c r="C4" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="18">
         <f>SUM(hatching!L14:L19)</f>
         <v>839913.93939393933</v>
       </c>
@@ -22322,7 +22334,7 @@
       <c r="J4" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="18">
         <f>839913.9394/5</f>
         <v>167982.78788000002</v>
       </c>
@@ -22337,7 +22349,7 @@
       <c r="C5" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="18">
         <f>SUM(hatching!L20:L25)</f>
         <v>841320</v>
       </c>
@@ -22358,7 +22370,7 @@
       <c r="J5" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="18">
         <f>841320/5</f>
         <v>168264</v>
       </c>
@@ -22373,7 +22385,7 @@
       <c r="C6" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="18">
         <f>SUM(hatching!L26:L27)</f>
         <v>850666.66666666674</v>
       </c>
@@ -22394,7 +22406,7 @@
       <c r="J6" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="18">
         <f>850666.6667/4</f>
         <v>212666.66667499999</v>
       </c>
@@ -22403,18 +22415,6 @@
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="M7" s="2"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <f>57*5</f>
-        <v>285</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <f>800-285</f>
-        <v>515</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>